<commit_message>
Fix bug in cosmed import
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/cosmed.xlsx
+++ b/tests/testthat/testdata/cosmed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\sciebo\Wissenschaft\R\spiro\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RH7765\sciebo - Nolte, Simon (rh7765@dshs-koeln.de)@dshs-koeln.sciebo.de\Wissenschaft\R\spiro\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB1A8EB-28FA-4CA5-A27C-A56308E0D36E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F31D8F6-D27F-4F52-ACCF-31CDED0CED9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5820" yWindow="4010" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daten" sheetId="2" r:id="rId1"/>
@@ -810,8 +810,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:BH80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1752,7 +1752,7 @@
         <v>95</v>
       </c>
       <c r="B7">
-        <v>71.5</v>
+        <v>67.099999999999994</v>
       </c>
       <c r="D7" t="s">
         <v>96</v>

</xml_diff>